<commit_message>
Atualização automática de VENANCIO_AIRES.xlsx
</commit_message>
<xml_diff>
--- a/VENANCIO_AIRES.xlsx
+++ b/VENANCIO_AIRES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6BB5D49-DE08-408A-9F76-27136EDF72D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9ED6FB53-02A0-410E-A02D-E0E27EFAB0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1341,7 +1341,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{51779A7A-A970-41B5-AFCC-E5B529AFDD56}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{4713B18D-6C5D-4ABA-9172-738C535CFA8D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1371,10 +1371,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{711E04D8-6F66-401E-961C-558D8320F12C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E97B5E04-3C4B-4264-B383-E0F16709E115}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1412,7 +1412,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A320854-7938-4AE5-94D7-3050306C1E65}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ADAC54F-B264-4F68-ABB8-78C8F4A8E21E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1475,7 +1475,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FB2A42C-1FBF-4DA2-8E10-CAFE916C34F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E64F858-F2AD-4A43-81DD-DC41E1E11179}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1494,7 +1494,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6D40D53-C25A-6778-E15E-0FF38B62A233}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2DDC731-AF7B-39F8-7CDD-7BBE7BDF6613}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1543,7 +1543,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF637F26-0352-4EC1-76CF-8DE8063B2451}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{098FFB62-7D30-F229-1DD4-4C9D267AD826}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1562,7 +1562,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F22D9B8F-32DC-E34A-5429-6C432C6D6C00}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78CD7E10-7BD0-B1E8-73F9-5A1461588565}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1593,7 +1593,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F178D506-DD1B-22BF-10BC-E7E673CDCA0A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CB68E51-38DF-75BA-D84A-47185F380343}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1624,7 +1624,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62FE181F-9B0A-7AA5-244C-08B4C5A0F93B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E443236-F69C-A45B-5921-6E685D8D5473}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1667,7 +1667,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0E9A217-53FA-4C61-BC53-CF79BC302434}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A436061-0A4A-4D19-81B7-26BC19E57B53}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1705,7 +1705,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9365EC9-B569-4FB7-A3BE-EEF033593271}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60FAA786-EEDC-4863-B30D-1600D44F97FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1748,7 +1748,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67DC3012-8AF9-4439-94B0-187C273A856E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B3D8342-39D6-4B87-A7DB-7DEBA4352BA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2061,7 +2061,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5273C8-5E17-455F-A213-568592189421}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D62AA0-B0AD-49FD-B670-1709AE0D1460}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>